<commit_message>
fix path to be input
</commit_message>
<xml_diff>
--- a/current/background_files/מיקום מקורי של הקבצים.xlsx
+++ b/current/background_files/מיקום מקורי של הקבצים.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Data\Forecast\Tools\creat_forecast_basic\current\background_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F2EF7A-FD2B-448E-A9E2-0C3290FC17DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69090208-AAFD-4FD4-A5EA-C0E833E30AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>מספר דירות לפי אזורים סטטיסטיים</t>
   </si>
@@ -643,13 +643,178 @@
   </si>
   <si>
     <t>pop_2020_cbs_muni</t>
+  </si>
+  <si>
+    <t>fix_cbs_data_230717.ipynb</t>
+  </si>
+  <si>
+    <t>קוד בשימוש</t>
+  </si>
+  <si>
+    <t>stat_11_cbs_2020_with_jtmt_fix.shp</t>
+  </si>
+  <si>
+    <t>from_sa_cbs_to_ta_jtmt.ipynb</t>
+  </si>
+  <si>
+    <r>
+      <t>W:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\M</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>odel Versions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF569CD6"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AZ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD16969"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>AZ_V4_230518_Published.shp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>W:\Data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\G</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IS\BaseLayers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\ב</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>נטל - מפי\BNTL 2022</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\J</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>erusalem Transportation.gdb</t>
+    </r>
+  </si>
+  <si>
+    <t>BLDG_Clip</t>
+  </si>
+  <si>
+    <t>POI_BLDG_Clip</t>
+  </si>
+  <si>
+    <t>taz_not_relevant_for_pop_2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -697,6 +862,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD7BA7D"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF569CD6"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -719,7 +898,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -728,6 +907,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -769,11 +951,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BF3968A-E6A6-4806-8293-4309D7C8C4A9}" name="טבלה1" displayName="טבלה1" ref="A1:B11" totalsRowShown="0">
-  <autoFilter ref="A1:B11" xr:uid="{5BF3968A-E6A6-4806-8293-4309D7C8C4A9}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5BF3968A-E6A6-4806-8293-4309D7C8C4A9}" name="טבלה1" displayName="טבלה1" ref="A1:C16" totalsRowShown="0">
+  <autoFilter ref="A1:C16" xr:uid="{5BF3968A-E6A6-4806-8293-4309D7C8C4A9}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{6BCCDF95-BDED-4C61-84E1-0F6B5F0AF51D}" name="שם קובץ"/>
     <tableColumn id="2" xr3:uid="{7D45C3C1-4937-4A6F-9B9E-60D2EF57A1C4}" name="מיקום מקורי" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{6288211B-151E-4E12-AEC8-F53A180119A7}" name="קוד בשימוש"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1042,113 +1225,204 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="75.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{889AC0C3-C22E-42A3-9737-B08BD70BA9FC}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{615BCA1A-5EA6-4880-A916-46219CF68507}"/>
+    <hyperlink ref="B16" r:id="rId3" xr:uid="{11FDAED8-DD6C-4698-9B1B-5DC280E10C7C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>